<commit_message>
Push new Dash Update with dataframe
</commit_message>
<xml_diff>
--- a/GWC/updated_GWTC.xlsx
+++ b/GWC/updated_GWTC.xlsx
@@ -8486,22 +8486,22 @@
         <v>27.3</v>
       </c>
       <c r="I64" t="n">
-        <v>-6</v>
+        <v>-5.9</v>
       </c>
       <c r="J64" t="n">
-        <v>11</v>
+        <v>10.8</v>
       </c>
       <c r="K64" t="n">
-        <v>19.3</v>
+        <v>19.2</v>
       </c>
       <c r="L64" t="n">
         <v>-6</v>
       </c>
       <c r="M64" t="n">
-        <v>5.6</v>
+        <v>5.5</v>
       </c>
       <c r="N64" t="n">
-        <v>8.800000000000001</v>
+        <v>8.9</v>
       </c>
       <c r="O64" t="n">
         <v>-0.6</v>
@@ -8510,7 +8510,7 @@
         <v>0.4</v>
       </c>
       <c r="Q64" t="n">
-        <v>1800</v>
+        <v>1900</v>
       </c>
       <c r="R64" t="n">
         <v>-1100</v>
@@ -8522,25 +8522,25 @@
         <v>0.05</v>
       </c>
       <c r="U64" t="n">
-        <v>-0.27</v>
+        <v>-0.26</v>
       </c>
       <c r="V64" t="n">
-        <v>0.26</v>
+        <v>0.25</v>
       </c>
       <c r="W64" t="n">
-        <v>46.6</v>
+        <v>46.5</v>
       </c>
       <c r="X64" t="n">
-        <v>-8</v>
+        <v>-7.8</v>
       </c>
       <c r="Y64" t="n">
-        <v>9.199999999999999</v>
+        <v>9.1</v>
       </c>
       <c r="Z64" t="n">
         <v>19.8</v>
       </c>
       <c r="AA64" t="n">
-        <v>-3.3</v>
+        <v>-3.2</v>
       </c>
       <c r="AB64" t="n">
         <v>3.6</v>
@@ -8571,10 +8571,10 @@
         <v>45</v>
       </c>
       <c r="AP64" t="n">
-        <v>-7.6</v>
+        <v>-7.5</v>
       </c>
       <c r="AQ64" t="n">
-        <v>8.6</v>
+        <v>8.699999999999999</v>
       </c>
     </row>
     <row r="65">
@@ -8610,40 +8610,40 @@
         </is>
       </c>
       <c r="H65" t="n">
-        <v>11.9</v>
+        <v>11.7</v>
       </c>
       <c r="I65" t="n">
-        <v>-1.8</v>
+        <v>-1.7</v>
       </c>
       <c r="J65" t="n">
         <v>3.3</v>
       </c>
       <c r="K65" t="n">
-        <v>8.199999999999999</v>
+        <v>8.4</v>
       </c>
       <c r="L65" t="n">
-        <v>-1.6</v>
+        <v>-1.7</v>
       </c>
       <c r="M65" t="n">
-        <v>1.4</v>
+        <v>1.3</v>
       </c>
       <c r="N65" t="n">
-        <v>17.5</v>
+        <v>17.4</v>
       </c>
       <c r="O65" t="n">
-        <v>-0.2</v>
+        <v>-0.3</v>
       </c>
       <c r="P65" t="n">
         <v>0.2</v>
       </c>
       <c r="Q65" t="n">
-        <v>650</v>
+        <v>640</v>
       </c>
       <c r="R65" t="n">
-        <v>-250</v>
+        <v>-260</v>
       </c>
       <c r="S65" t="n">
-        <v>190</v>
+        <v>200</v>
       </c>
       <c r="T65" t="n">
         <v>0.16</v>
@@ -8658,19 +8658,19 @@
         <v>20.1</v>
       </c>
       <c r="X65" t="n">
-        <v>-0.96</v>
+        <v>-0.95</v>
       </c>
       <c r="Y65" t="n">
-        <v>1.7</v>
+        <v>1.64</v>
       </c>
       <c r="Z65" t="n">
-        <v>8.550000000000001</v>
+        <v>8.56</v>
       </c>
       <c r="AA65" t="n">
-        <v>-0.27</v>
+        <v>-0.28</v>
       </c>
       <c r="AB65" t="n">
-        <v>0.38</v>
+        <v>0.41</v>
       </c>
       <c r="AC65" t="inlineStr"/>
       <c r="AD65" t="inlineStr"/>
@@ -8695,13 +8695,13 @@
       <c r="AM65" t="inlineStr"/>
       <c r="AN65" t="inlineStr"/>
       <c r="AO65" t="n">
-        <v>19.21</v>
+        <v>19.18</v>
       </c>
       <c r="AP65" t="n">
-        <v>-0.95</v>
+        <v>-0.93</v>
       </c>
       <c r="AQ65" t="n">
-        <v>1.79</v>
+        <v>1.71</v>
       </c>
     </row>
     <row r="66">
@@ -8867,7 +8867,7 @@
         <v>12.1</v>
       </c>
       <c r="I67" t="n">
-        <v>-2.3</v>
+        <v>-2.2</v>
       </c>
       <c r="J67" t="n">
         <v>4.6</v>
@@ -8912,10 +8912,10 @@
         <v>19.8</v>
       </c>
       <c r="X67" t="n">
-        <v>-0.9399999999999999</v>
+        <v>-0.93</v>
       </c>
       <c r="Y67" t="n">
-        <v>2.69</v>
+        <v>2.7</v>
       </c>
       <c r="Z67" t="n">
         <v>8.33</v>
@@ -8952,10 +8952,10 @@
         <v>18.87</v>
       </c>
       <c r="AP67" t="n">
-        <v>-0.9399999999999999</v>
+        <v>-0.93</v>
       </c>
       <c r="AQ67" t="n">
-        <v>2.8</v>
+        <v>2.81</v>
       </c>
     </row>
     <row r="68">
@@ -9024,7 +9024,7 @@
         <v>-160</v>
       </c>
       <c r="S68" t="n">
-        <v>250</v>
+        <v>240</v>
       </c>
       <c r="T68" t="n">
         <v>0</v>
@@ -9045,7 +9045,7 @@
         <v>2.2</v>
       </c>
       <c r="Z68" t="n">
-        <v>4.32</v>
+        <v>4.31</v>
       </c>
       <c r="AA68" t="n">
         <v>-0.17</v>
@@ -9511,7 +9511,7 @@
         <v>1.44</v>
       </c>
       <c r="L72" t="n">
-        <v>-0.29</v>
+        <v>-0.28</v>
       </c>
       <c r="M72" t="n">
         <v>0.85</v>
@@ -9541,7 +9541,7 @@
         <v>-0.42</v>
       </c>
       <c r="V72" t="n">
-        <v>0.24</v>
+        <v>0.23</v>
       </c>
       <c r="W72" t="n">
         <v>7.34</v>
@@ -9550,7 +9550,7 @@
         <v>-1.7</v>
       </c>
       <c r="Y72" t="n">
-        <v>1.8</v>
+        <v>1.7</v>
       </c>
       <c r="Z72" t="n">
         <v>2.43</v>
@@ -9756,19 +9756,19 @@
         <v>34.5</v>
       </c>
       <c r="I74" t="n">
-        <v>-3.2</v>
+        <v>-3.1</v>
       </c>
       <c r="J74" t="n">
         <v>9.9</v>
       </c>
       <c r="K74" t="n">
-        <v>28.9</v>
+        <v>29</v>
       </c>
       <c r="L74" t="n">
         <v>-9.300000000000001</v>
       </c>
       <c r="M74" t="n">
-        <v>3.4</v>
+        <v>3.3</v>
       </c>
       <c r="N74" t="n">
         <v>26.8</v>
@@ -9780,13 +9780,13 @@
         <v>0.2</v>
       </c>
       <c r="Q74" t="n">
-        <v>900</v>
+        <v>890</v>
       </c>
       <c r="R74" t="n">
-        <v>-380</v>
+        <v>-370</v>
       </c>
       <c r="S74" t="n">
-        <v>290</v>
+        <v>260</v>
       </c>
       <c r="T74" t="n">
         <v>0.11</v>
@@ -9798,13 +9798,13 @@
         <v>0.11</v>
       </c>
       <c r="W74" t="n">
-        <v>63.4</v>
+        <v>63.5</v>
       </c>
       <c r="X74" t="n">
-        <v>-3.6</v>
+        <v>-3.4</v>
       </c>
       <c r="Y74" t="n">
-        <v>4.3</v>
+        <v>4.5</v>
       </c>
       <c r="Z74" t="n">
         <v>27.2</v>
@@ -9838,13 +9838,13 @@
       <c r="AM74" t="inlineStr"/>
       <c r="AN74" t="inlineStr"/>
       <c r="AO74" t="n">
-        <v>60.3</v>
+        <v>60.2</v>
       </c>
       <c r="AP74" t="n">
-        <v>-3.3</v>
+        <v>-3.2</v>
       </c>
       <c r="AQ74" t="n">
-        <v>4</v>
+        <v>4.1</v>
       </c>
     </row>
     <row r="75">
@@ -10007,22 +10007,22 @@
         </is>
       </c>
       <c r="H76" t="n">
-        <v>37.8</v>
+        <v>37.7</v>
       </c>
       <c r="I76" t="n">
         <v>-6.2</v>
       </c>
       <c r="J76" t="n">
-        <v>9.199999999999999</v>
+        <v>9.300000000000001</v>
       </c>
       <c r="K76" t="n">
         <v>27.4</v>
       </c>
       <c r="L76" t="n">
-        <v>-7.4</v>
+        <v>-7.3</v>
       </c>
       <c r="M76" t="n">
-        <v>6.1</v>
+        <v>6.3</v>
       </c>
       <c r="N76" t="n">
         <v>10.8</v>
@@ -10040,7 +10040,7 @@
         <v>-850</v>
       </c>
       <c r="S76" t="n">
-        <v>1000</v>
+        <v>1020</v>
       </c>
       <c r="T76" t="n">
         <v>-0.07000000000000001</v>
@@ -10049,16 +10049,16 @@
         <v>-0.27</v>
       </c>
       <c r="V76" t="n">
-        <v>0.22</v>
+        <v>0.21</v>
       </c>
       <c r="W76" t="n">
-        <v>65.19999999999999</v>
+        <v>65.09999999999999</v>
       </c>
       <c r="X76" t="n">
         <v>-6.8</v>
       </c>
       <c r="Y76" t="n">
-        <v>7.8</v>
+        <v>8.1</v>
       </c>
       <c r="Z76" t="n">
         <v>27.7</v>
@@ -10067,7 +10067,7 @@
         <v>-3.1</v>
       </c>
       <c r="AB76" t="n">
-        <v>3.6</v>
+        <v>3.7</v>
       </c>
       <c r="AC76" t="inlineStr"/>
       <c r="AD76" t="inlineStr"/>
@@ -10098,7 +10098,7 @@
         <v>-6.4</v>
       </c>
       <c r="AQ76" t="n">
-        <v>7.3</v>
+        <v>7.5</v>
       </c>
     </row>
     <row r="77">
@@ -10140,16 +10140,16 @@
         <v>-30</v>
       </c>
       <c r="J77" t="n">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="K77" t="n">
         <v>12.3</v>
       </c>
       <c r="L77" t="n">
-        <v>-5.7</v>
+        <v>-5.5</v>
       </c>
       <c r="M77" t="n">
-        <v>9</v>
+        <v>9.199999999999999</v>
       </c>
       <c r="N77" t="n">
         <v>7.4</v>
@@ -10164,7 +10164,7 @@
         <v>4100</v>
       </c>
       <c r="R77" t="n">
-        <v>-1900</v>
+        <v>-2000</v>
       </c>
       <c r="S77" t="n">
         <v>4400</v>
@@ -10173,28 +10173,28 @@
         <v>0.45</v>
       </c>
       <c r="U77" t="n">
-        <v>-0.44</v>
+        <v>-0.46</v>
       </c>
       <c r="V77" t="n">
-        <v>0.43</v>
+        <v>0.42</v>
       </c>
       <c r="W77" t="n">
         <v>63.3</v>
       </c>
       <c r="X77" t="n">
-        <v>-25</v>
+        <v>-26</v>
       </c>
       <c r="Y77" t="n">
         <v>100</v>
       </c>
       <c r="Z77" t="n">
-        <v>19.6</v>
+        <v>19.8</v>
       </c>
       <c r="AA77" t="n">
-        <v>-5.1</v>
+        <v>-5.2</v>
       </c>
       <c r="AB77" t="n">
-        <v>10.7</v>
+        <v>10.5</v>
       </c>
       <c r="AC77" t="inlineStr"/>
       <c r="AD77" t="inlineStr"/>
@@ -10203,10 +10203,10 @@
         <v>0.66</v>
       </c>
       <c r="AG77" t="n">
-        <v>-0.28</v>
+        <v>-0.29</v>
       </c>
       <c r="AH77" t="n">
-        <v>0.54</v>
+        <v>0.53</v>
       </c>
       <c r="AI77" t="n">
         <v>4.8</v>
@@ -10222,10 +10222,10 @@
         <v>61</v>
       </c>
       <c r="AP77" t="n">
-        <v>-25</v>
+        <v>-26</v>
       </c>
       <c r="AQ77" t="n">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="78">
@@ -11029,16 +11029,16 @@
         <v>-4.5</v>
       </c>
       <c r="J84" t="n">
-        <v>6.9</v>
+        <v>6.7</v>
       </c>
       <c r="K84" t="n">
-        <v>32.5</v>
+        <v>32.7</v>
       </c>
       <c r="L84" t="n">
         <v>-7.2</v>
       </c>
       <c r="M84" t="n">
-        <v>5</v>
+        <v>4.8</v>
       </c>
       <c r="N84" t="n">
         <v>20</v>
@@ -11053,25 +11053,25 @@
         <v>1710</v>
       </c>
       <c r="R84" t="n">
-        <v>-640</v>
+        <v>-650</v>
       </c>
       <c r="S84" t="n">
-        <v>490</v>
+        <v>500</v>
       </c>
       <c r="T84" t="n">
         <v>0.1</v>
       </c>
       <c r="U84" t="n">
-        <v>-0.15</v>
+        <v>-0.16</v>
       </c>
       <c r="V84" t="n">
         <v>0.15</v>
       </c>
       <c r="W84" t="n">
-        <v>72.5</v>
+        <v>72.7</v>
       </c>
       <c r="X84" t="n">
-        <v>-5.1</v>
+        <v>-5.3</v>
       </c>
       <c r="Y84" t="n">
         <v>7.2</v>
@@ -11080,10 +11080,10 @@
         <v>31.1</v>
       </c>
       <c r="AA84" t="n">
-        <v>-2.6</v>
+        <v>-2.7</v>
       </c>
       <c r="AB84" t="n">
-        <v>3.2</v>
+        <v>3.3</v>
       </c>
       <c r="AC84" t="inlineStr"/>
       <c r="AD84" t="inlineStr"/>
@@ -11108,13 +11108,13 @@
       <c r="AM84" t="inlineStr"/>
       <c r="AN84" t="inlineStr"/>
       <c r="AO84" t="n">
-        <v>68.59999999999999</v>
+        <v>68.7</v>
       </c>
       <c r="AP84" t="n">
-        <v>-4.7</v>
+        <v>-4.8</v>
       </c>
       <c r="AQ84" t="n">
-        <v>6.6</v>
+        <v>6.7</v>
       </c>
     </row>
     <row r="85">
@@ -11531,79 +11531,79 @@
         </is>
       </c>
       <c r="H88" t="n">
-        <v>36.4</v>
+        <v>60</v>
       </c>
       <c r="I88" t="n">
-        <v>-9.6</v>
+        <v>-29</v>
       </c>
       <c r="J88" t="n">
-        <v>11.2</v>
+        <v>166</v>
       </c>
       <c r="K88" t="n">
-        <v>13.8</v>
+        <v>24</v>
       </c>
       <c r="L88" t="n">
-        <v>-3.3</v>
+        <v>-13</v>
       </c>
       <c r="M88" t="n">
-        <v>7.2</v>
+        <v>36</v>
       </c>
       <c r="N88" t="n">
-        <v>7.1</v>
+        <v>4.7</v>
       </c>
       <c r="O88" t="n">
-        <v>-0.5</v>
+        <v>-2.9</v>
       </c>
       <c r="P88" t="n">
-        <v>0.5</v>
+        <v>2.5</v>
       </c>
       <c r="Q88" t="n">
-        <v>5400</v>
+        <v>7100</v>
       </c>
       <c r="R88" t="n">
-        <v>-2600</v>
+        <v>-4400</v>
       </c>
       <c r="S88" t="n">
-        <v>2700</v>
+        <v>13900</v>
       </c>
       <c r="T88" t="n">
-        <v>0.65</v>
+        <v>0.16</v>
       </c>
       <c r="U88" t="n">
-        <v>-0.21</v>
+        <v>-0.49</v>
       </c>
       <c r="V88" t="n">
-        <v>0.17</v>
+        <v>0.58</v>
       </c>
       <c r="W88" t="n">
-        <v>50.2</v>
+        <v>84</v>
       </c>
       <c r="X88" t="n">
-        <v>-8.5</v>
+        <v>-48</v>
       </c>
       <c r="Y88" t="n">
-        <v>10.9</v>
+        <v>169</v>
       </c>
       <c r="Z88" t="n">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="AA88" t="n">
-        <v>-2.8</v>
+        <v>-18</v>
       </c>
       <c r="AB88" t="n">
-        <v>4.8</v>
+        <v>44</v>
       </c>
       <c r="AC88" t="inlineStr"/>
       <c r="AD88" t="inlineStr"/>
       <c r="AE88" t="inlineStr"/>
       <c r="AF88" t="n">
-        <v>0.83</v>
+        <v>1.04</v>
       </c>
       <c r="AG88" t="n">
-        <v>-0.35</v>
+        <v>-0.57</v>
       </c>
       <c r="AH88" t="n">
-        <v>0.32</v>
+        <v>1.47</v>
       </c>
       <c r="AI88" t="n">
         <v>2.4</v>
@@ -11616,13 +11616,13 @@
       <c r="AM88" t="inlineStr"/>
       <c r="AN88" t="inlineStr"/>
       <c r="AO88" t="n">
-        <v>47.4</v>
+        <v>88</v>
       </c>
       <c r="AP88" t="n">
-        <v>-7.7</v>
+        <v>-47</v>
       </c>
       <c r="AQ88" t="n">
-        <v>11.1</v>
+        <v>169</v>
       </c>
     </row>
     <row r="89">
@@ -11800,7 +11800,7 @@
         <v>-2.9</v>
       </c>
       <c r="M90" t="n">
-        <v>1.9</v>
+        <v>2</v>
       </c>
       <c r="N90" t="n">
         <v>10.3</v>
@@ -11818,7 +11818,7 @@
         <v>-440</v>
       </c>
       <c r="S90" t="n">
-        <v>470</v>
+        <v>480</v>
       </c>
       <c r="T90" t="n">
         <v>0.13</v>
@@ -11912,79 +11912,79 @@
         </is>
       </c>
       <c r="H91" t="n">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="I91" t="n">
-        <v>-18</v>
+        <v>-22</v>
       </c>
       <c r="J91" t="n">
-        <v>48</v>
+        <v>130</v>
       </c>
       <c r="K91" t="n">
-        <v>14</v>
+        <v>11.3</v>
       </c>
       <c r="L91" t="n">
-        <v>-8.699999999999999</v>
+        <v>-6</v>
       </c>
       <c r="M91" t="n">
-        <v>16.8</v>
+        <v>24.3</v>
       </c>
       <c r="N91" t="n">
-        <v>6</v>
+        <v>4.5</v>
       </c>
       <c r="O91" t="n">
-        <v>-1.2</v>
+        <v>-3</v>
       </c>
       <c r="P91" t="n">
-        <v>1.7</v>
+        <v>2.7</v>
       </c>
       <c r="Q91" t="n">
-        <v>3600</v>
+        <v>3500</v>
       </c>
       <c r="R91" t="n">
-        <v>-2000</v>
+        <v>-2200</v>
       </c>
       <c r="S91" t="n">
-        <v>7000</v>
+        <v>12500</v>
       </c>
       <c r="T91" t="n">
-        <v>0.24</v>
+        <v>0.27</v>
       </c>
       <c r="U91" t="n">
-        <v>-0.51</v>
+        <v>-0.58</v>
       </c>
       <c r="V91" t="n">
-        <v>0.45</v>
+        <v>0.54</v>
       </c>
       <c r="W91" t="n">
-        <v>48</v>
+        <v>49.3</v>
       </c>
       <c r="X91" t="n">
-        <v>-27</v>
+        <v>-22</v>
       </c>
       <c r="Y91" t="n">
-        <v>37</v>
+        <v>132</v>
       </c>
       <c r="Z91" t="n">
-        <v>15.5</v>
+        <v>15</v>
       </c>
       <c r="AA91" t="n">
-        <v>-3.7</v>
+        <v>-4</v>
       </c>
       <c r="AB91" t="n">
-        <v>15.7</v>
+        <v>29.5</v>
       </c>
       <c r="AC91" t="inlineStr"/>
       <c r="AD91" t="inlineStr"/>
       <c r="AE91" t="inlineStr"/>
       <c r="AF91" t="n">
-        <v>0.6</v>
+        <v>0.59</v>
       </c>
       <c r="AG91" t="n">
-        <v>-0.3</v>
+        <v>-0.32</v>
       </c>
       <c r="AH91" t="n">
-        <v>0.84</v>
+        <v>1.43</v>
       </c>
       <c r="AI91" t="n">
         <v>140</v>
@@ -11997,13 +11997,13 @@
       <c r="AM91" t="inlineStr"/>
       <c r="AN91" t="inlineStr"/>
       <c r="AO91" t="n">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="AP91" t="n">
-        <v>-26</v>
+        <v>-22</v>
       </c>
       <c r="AQ91" t="n">
-        <v>38</v>
+        <v>132</v>
       </c>
     </row>
   </sheetData>

</xml_diff>